<commit_message>
[Update] add erros different kinds and small errors
</commit_message>
<xml_diff>
--- a/src/count_events.xlsx
+++ b/src/count_events.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26501"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luisc\Master\Thesis\Master_thesis\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C08D04A6-3754-42B7-BBDF-1BC229940C4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D19A88A-9BB6-47EA-A1DE-35025271D0ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4590" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="13900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -536,10 +536,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B4:Y11"/>
+  <dimension ref="B4:Y15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V6" sqref="V6"/>
+      <selection activeCell="C9" sqref="C9:C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -883,6 +883,26 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
       <c r="Y11" s="8"/>
+    </row>
+    <row r="15" spans="2:25" x14ac:dyDescent="0.35">
+      <c r="E15">
+        <v>2000</v>
+      </c>
+      <c r="F15">
+        <v>2006</v>
+      </c>
+      <c r="G15">
+        <v>2009</v>
+      </c>
+      <c r="H15">
+        <v>2010</v>
+      </c>
+      <c r="I15">
+        <v>2013</v>
+      </c>
+      <c r="J15">
+        <v>2014</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>